<commit_message>
fix some bug and update README.md
</commit_message>
<xml_diff>
--- a/output/金門縣/2020_山地原住民立委_各村里得票數_金門縣.xlsx
+++ b/output/金門縣/2020_山地原住民立委_各村里得票數_金門縣.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,67 +665,67 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N6" t="n">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="S6" t="n">
-        <v>38</v>
+        <v>213</v>
       </c>
       <c r="T6" t="n">
-        <v>92</v>
+        <v>366</v>
       </c>
       <c r="U6" t="n">
-        <v>58.7</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">　南竿鄉</t>
+          <t xml:space="preserve">　金城鎮</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -733,13 +733,13 @@
         <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -748,50 +748,50 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" t="n">
         <v>1</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>6</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
       <c r="N7" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O7" t="n">
         <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="S7" t="n">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="T7" t="n">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="U7" t="n">
-        <v>53.49</v>
+        <v>37.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>介壽村</t>
+          <t>東門里</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -816,51 +816,51 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>復興村、福沃村</t>
+          <t>西門里</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -887,45 +887,45 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>54.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>清水村、珠螺村</t>
+          <t>南門里</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -952,54 +952,54 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
-        <v>68.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>仁愛村、津沙村、馬祖村、四維村</t>
+          <t>北門里</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1008,52 +1008,52 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
+        <v>3</v>
+      </c>
+      <c r="M11" t="n">
         <v>1</v>
       </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
       <c r="N11" t="n">
+        <v>27</v>
+      </c>
+      <c r="O11" t="n">
         <v>1</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
       <c r="P11" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="S11" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="T11" t="n">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="U11" t="n">
-        <v>16.67</v>
+        <v>37.84</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">　北竿鄉</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>古城里</t>
+        </is>
+      </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1082,41 +1082,41 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
-        <v>65.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>塘岐村、后沃村</t>
+          <t>金水里</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1147,41 +1147,41 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>70.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>橋仔村、芹壁村、坂里村、白沙村</t>
+          <t>珠沙里</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1194,179 +1194,179 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>賢庵里</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　金沙鎮</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>11</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>3</v>
       </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>3</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>3</v>
-      </c>
-      <c r="S14" t="n">
-        <v>3</v>
-      </c>
-      <c r="T14" t="n">
-        <v>6</v>
-      </c>
-      <c r="U14" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">　莒光鄉</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="J16" t="n">
+        <v>4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
         <v>5</v>
       </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>3</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>10</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="n">
-        <v>10</v>
-      </c>
-      <c r="S15" t="n">
-        <v>7</v>
-      </c>
-      <c r="T15" t="n">
-        <v>17</v>
-      </c>
-      <c r="U15" t="n">
-        <v>58.82</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>青帆村、田沃村、西坵村</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>2</v>
-      </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="S16" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="T16" t="n">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="U16" t="n">
         <v>55.56</v>
@@ -1376,11 +1376,11 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>福正村、大坪村</t>
+          <t>汶沙里</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1389,63 +1389,63 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
+        <v>11</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
         <v>3</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="S17" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="T17" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="U17" t="n">
-        <v>62.5</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">　東引鄉</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>三山里</t>
+        </is>
+      </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1478,93 +1478,2043 @@
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="U18" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>中柳村、樂華村</t>
+          <t>大洋里</t>
         </is>
       </c>
       <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>光前里</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>何斗里</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>西園里</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>官嶼里</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>浦山里</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　金湖鎮</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>21</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>9</v>
+      </c>
+      <c r="J25" t="n">
+        <v>8</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>8</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>51</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>51</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>51</v>
+      </c>
+      <c r="S25" t="n">
+        <v>72</v>
+      </c>
+      <c r="T25" t="n">
+        <v>123</v>
+      </c>
+      <c r="U25" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>新市里</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>21</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>9</v>
+      </c>
+      <c r="J26" t="n">
+        <v>8</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>8</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>51</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>51</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>51</v>
+      </c>
+      <c r="S26" t="n">
+        <v>72</v>
+      </c>
+      <c r="T26" t="n">
+        <v>123</v>
+      </c>
+      <c r="U26" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>山外里</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>正義里</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>料羅里</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>瓊林里</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>新湖里</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>溪湖里</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>蓮庵里</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　金寧鄉</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" t="n">
         <v>1</v>
       </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>4</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="n">
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>15</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>3</v>
+      </c>
+      <c r="J34" t="n">
         <v>5</v>
       </c>
-      <c r="O19" t="n">
+      <c r="K34" t="n">
         <v>1</v>
       </c>
-      <c r="P19" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="n">
-        <v>6</v>
-      </c>
-      <c r="S19" t="n">
+      <c r="L34" t="n">
         <v>3</v>
       </c>
-      <c r="T19" t="n">
+      <c r="M34" t="n">
+        <v>2</v>
+      </c>
+      <c r="N34" t="n">
+        <v>38</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>39</v>
+      </c>
+      <c r="S34" t="n">
+        <v>62</v>
+      </c>
+      <c r="T34" t="n">
+        <v>101</v>
+      </c>
+      <c r="U34" t="n">
+        <v>38.61</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>古寧村</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>安美村</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>15</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>3</v>
+      </c>
+      <c r="J36" t="n">
+        <v>5</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>3</v>
+      </c>
+      <c r="M36" t="n">
+        <v>2</v>
+      </c>
+      <c r="N36" t="n">
+        <v>38</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>39</v>
+      </c>
+      <c r="S36" t="n">
+        <v>62</v>
+      </c>
+      <c r="T36" t="n">
+        <v>101</v>
+      </c>
+      <c r="U36" t="n">
+        <v>38.61</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>后盤村</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>湖埔村</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>榜林村</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>盤山村</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　烈嶼鄉</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>2</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
         <v>9</v>
       </c>
-      <c r="U19" t="n">
-        <v>66.67</v>
+      <c r="O41" t="n">
+        <v>1</v>
+      </c>
+      <c r="P41" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>10</v>
+      </c>
+      <c r="S41" t="n">
+        <v>11</v>
+      </c>
+      <c r="T41" t="n">
+        <v>21</v>
+      </c>
+      <c r="U41" t="n">
+        <v>47.62</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>上岐村</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>上林村</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>西口村</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>林湖村</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>2</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>9</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1</v>
+      </c>
+      <c r="P45" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>10</v>
+      </c>
+      <c r="S45" t="n">
+        <v>11</v>
+      </c>
+      <c r="T45" t="n">
+        <v>21</v>
+      </c>
+      <c r="U45" t="n">
+        <v>47.62</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>黃埔村</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　烏坵鄉</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>2</v>
+      </c>
+      <c r="T47" t="n">
+        <v>2</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>大坵村</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>2</v>
+      </c>
+      <c r="T48" t="n">
+        <v>2</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>小坵村</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>